<commit_message>
Connecting logging to the project
</commit_message>
<xml_diff>
--- a/src/main/resources/statisticInfo.xlsx
+++ b/src/main/resources/statisticInfo.xlsx
@@ -32,6 +32,18 @@
     <t>Названия университетов</t>
   </si>
   <si>
+    <t>MATHEMATICS</t>
+  </si>
+  <si>
+    <t>Казанский Университет Вычислений</t>
+  </si>
+  <si>
+    <t>MEDICINE</t>
+  </si>
+  <si>
+    <t>Московский Государственный Медицинский Университет, Тамбовский Университет Медицины, Самарский Медицинский Институт</t>
+  </si>
+  <si>
     <t>PHYSICS</t>
   </si>
   <si>
@@ -42,18 +54,6 @@
   </si>
   <si>
     <t>Воронежский Литературно-Переводческий Университет</t>
-  </si>
-  <si>
-    <t>MEDICINE</t>
-  </si>
-  <si>
-    <t>Московский Государственный Медицинский Университет, Тамбовский Университет Медицины, Самарский Медицинский Институт</t>
-  </si>
-  <si>
-    <t>MATHEMATICS</t>
-  </si>
-  <si>
-    <t>Казанский Университет Вычислений</t>
   </si>
 </sst>
 </file>
@@ -138,12 +138,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.59375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="26.79296875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="36.72265625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="41.3984375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="110.01953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="7.796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="27.7890625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="37.671875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="42.6328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="124.859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -174,13 +174,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="n" s="2">
-        <v>4.538</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n" s="2">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F2" t="s" s="2">
         <v>7</v>
@@ -194,13 +194,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>0.0</v>
+        <v>4.333</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F3" t="s" s="2">
         <v>9</v>
@@ -214,13 +214,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>4.333</v>
+        <v>4.538</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="F4" t="s" s="2">
         <v>11</v>

</xml_diff>

<commit_message>
Marshalling and serialization functionality completed
</commit_message>
<xml_diff>
--- a/src/main/resources/statisticInfo.xlsx
+++ b/src/main/resources/statisticInfo.xlsx
@@ -32,28 +32,28 @@
     <t>Названия университетов</t>
   </si>
   <si>
+    <t>PHYSICS</t>
+  </si>
+  <si>
+    <t>Московский Выдуманный Университет, Московский Придуманный Институт</t>
+  </si>
+  <si>
+    <t>LINGUISTICS</t>
+  </si>
+  <si>
+    <t>Воронежский Литературно-Переводческий Университет</t>
+  </si>
+  <si>
+    <t>MEDICINE</t>
+  </si>
+  <si>
+    <t>Московский Государственный Медицинский Университет, Тамбовский Университет Медицины, Самарский Медицинский Институт</t>
+  </si>
+  <si>
     <t>MATHEMATICS</t>
   </si>
   <si>
     <t>Казанский Университет Вычислений</t>
-  </si>
-  <si>
-    <t>MEDICINE</t>
-  </si>
-  <si>
-    <t>Московский Государственный Медицинский Университет, Тамбовский Университет Медицины, Самарский Медицинский Институт</t>
-  </si>
-  <si>
-    <t>LINGUISTICS</t>
-  </si>
-  <si>
-    <t>Воронежский Литературно-Переводческий Университет</t>
-  </si>
-  <si>
-    <t>PHYSICS</t>
-  </si>
-  <si>
-    <t>Московский Выдуманный Университет, Московский Придуманный Институт</t>
   </si>
 </sst>
 </file>
@@ -174,13 +174,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="n" s="2">
-        <v>0.0</v>
+        <v>4.538</v>
       </c>
       <c r="D2" t="n" s="2">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F2" t="s" s="2">
         <v>7</v>
@@ -194,13 +194,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>4.333</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3" t="s" s="2">
         <v>9</v>
@@ -214,13 +214,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>0.0</v>
+        <v>4.333</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F4" t="s" s="2">
         <v>11</v>
@@ -234,13 +234,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>4.538</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F5" t="s" s="2">
         <v>13</v>

</xml_diff>